<commit_message>
Corrijo algoritmos y memoria
</commit_message>
<xml_diff>
--- a/tablas/medidas_por_dataset.xlsx
+++ b/tablas/medidas_por_dataset.xlsx
@@ -98,10 +98,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -168,7 +167,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -177,15 +176,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -208,11 +203,11 @@
   </sheetPr>
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K57" activeCellId="0" sqref="K57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K55" activeCellId="0" sqref="K55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -259,7 +254,7 @@
       <c r="M3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="N3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -267,43 +262,43 @@
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="0" t="n">
         <v>417</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="0" t="n">
         <v>87</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="0" t="n">
         <v>323</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="2" t="n">
         <v>0.827380952380952</v>
       </c>
-      <c r="G4" s="3" t="n">
+      <c r="G4" s="2" t="n">
         <v>0.822485207100592</v>
       </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="2" t="n">
         <v>0.787804878048781</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="2" t="n">
         <v>0.824925816023739</v>
       </c>
-      <c r="J4" s="3" t="n">
+      <c r="J4" s="2" t="n">
         <v>0.806979280261723</v>
       </c>
-      <c r="K4" s="3" t="n">
+      <c r="K4" s="2" t="n">
         <v>0.609863207309071</v>
       </c>
-      <c r="L4" s="3" t="n">
+      <c r="L4" s="2" t="n">
         <v>0.804958295986076</v>
       </c>
-      <c r="M4" s="3" t="n">
+      <c r="M4" s="2" t="n">
         <v>0.808647013635491</v>
       </c>
-      <c r="N4" s="0" t="n">
+      <c r="N4" s="1" t="n">
         <v>69</v>
       </c>
     </row>
@@ -323,31 +318,31 @@
       <c r="E5" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F5" s="2" t="n">
         <v>0.91869918699187</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="2" t="n">
         <v>0.904</v>
       </c>
-      <c r="H5" s="4" t="n">
+      <c r="H5" s="2" t="n">
         <v>0.973333333333333</v>
       </c>
-      <c r="I5" s="4" t="n">
+      <c r="I5" s="2" t="n">
         <v>0.911290322580645</v>
       </c>
-      <c r="J5" s="4" t="n">
+      <c r="J5" s="2" t="n">
         <v>0.8455</v>
       </c>
-      <c r="K5" s="4" t="n">
+      <c r="K5" s="2" t="n">
         <v>0.794</v>
       </c>
-      <c r="L5" s="4" t="n">
+      <c r="L5" s="2" t="n">
         <v>0.938026296717386</v>
       </c>
-      <c r="M5" s="4" t="n">
+      <c r="M5" s="2" t="n">
         <v>0.959101333333333</v>
       </c>
-      <c r="N5" s="0" t="n">
+      <c r="N5" s="1" t="n">
         <v>109</v>
       </c>
     </row>
@@ -367,31 +362,31 @@
       <c r="E6" s="0" t="n">
         <v>2158</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="F6" s="2" t="n">
         <v>0.54052165812762</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="2" t="n">
         <v>0.518196025898638</v>
       </c>
-      <c r="H6" s="4" t="n">
+      <c r="H6" s="2" t="n">
         <v>0.94570422147614</v>
       </c>
-      <c r="I6" s="4" t="n">
+      <c r="I6" s="2" t="n">
         <v>0.529123446939473</v>
       </c>
-      <c r="J6" s="4" t="n">
+      <c r="J6" s="2" t="n">
         <v>0.898792169929196</v>
       </c>
-      <c r="K6" s="4" t="n">
+      <c r="K6" s="2" t="n">
         <v>0.472454694740885</v>
       </c>
-      <c r="L6" s="4" t="n">
+      <c r="L6" s="2" t="n">
         <v>0.700042976712503</v>
       </c>
-      <c r="M6" s="4" t="n">
+      <c r="M6" s="2" t="n">
         <v>0.75078890703015</v>
       </c>
-      <c r="N6" s="0" t="n">
+      <c r="N6" s="1" t="n">
         <v>2689</v>
       </c>
     </row>
@@ -411,31 +406,31 @@
       <c r="E7" s="0" t="n">
         <v>5631</v>
       </c>
-      <c r="F7" s="4" t="n">
+      <c r="F7" s="2" t="n">
         <v>0.793861487587909</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G7" s="2" t="n">
         <v>0.751675780560946</v>
       </c>
-      <c r="H7" s="4" t="n">
+      <c r="H7" s="2" t="n">
         <v>0.86203671955363</v>
       </c>
-      <c r="I7" s="4" t="n">
+      <c r="I7" s="2" t="n">
         <v>0.772192900989875</v>
       </c>
-      <c r="J7" s="4" t="n">
+      <c r="J7" s="2" t="n">
         <v>0.816333984696021</v>
       </c>
-      <c r="K7" s="4" t="n">
+      <c r="K7" s="2" t="n">
         <v>0.618530453487015</v>
       </c>
-      <c r="L7" s="4" t="n">
+      <c r="L7" s="2" t="n">
         <v>0.804967157120507</v>
       </c>
-      <c r="M7" s="4" t="n">
+      <c r="M7" s="2" t="n">
         <v>0.844448399600512</v>
       </c>
-      <c r="N7" s="0" t="n">
+      <c r="N7" s="1" t="n">
         <v>5042</v>
       </c>
     </row>
@@ -484,7 +479,7 @@
       <c r="M12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N12" s="0" t="s">
+      <c r="N12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -492,43 +487,43 @@
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" s="0" t="n">
         <v>455</v>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="C13" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D13" s="0" t="n">
         <v>339</v>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E13" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="F13" s="3" t="n">
+      <c r="F13" s="2" t="n">
         <v>0.865019011406844</v>
       </c>
-      <c r="G13" s="3" t="n">
+      <c r="G13" s="2" t="n">
         <v>0.895669291338582</v>
       </c>
-      <c r="H13" s="3" t="n">
+      <c r="H13" s="2" t="n">
         <v>0.826829268292683</v>
       </c>
-      <c r="I13" s="3" t="n">
+      <c r="I13" s="2" t="n">
         <v>0.880077369439072</v>
       </c>
-      <c r="J13" s="3" t="n">
+      <c r="J13" s="2" t="n">
         <v>0.864923747276688</v>
       </c>
-      <c r="K13" s="3" t="n">
+      <c r="K13" s="2" t="n">
         <v>0.725571124118844</v>
       </c>
-      <c r="L13" s="3" t="n">
+      <c r="L13" s="2" t="n">
         <v>0.860561203395613</v>
       </c>
-      <c r="M13" s="3" t="n">
+      <c r="M13" s="2" t="n">
         <v>0.922532168235068</v>
       </c>
-      <c r="N13" s="0" t="n">
+      <c r="N13" s="1" t="n">
         <v>100</v>
       </c>
     </row>
@@ -548,31 +543,31 @@
       <c r="E14" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" s="2" t="n">
         <v>0.916342412451362</v>
       </c>
-      <c r="G14" s="4" t="n">
+      <c r="G14" s="2" t="n">
         <v>0.942</v>
       </c>
-      <c r="H14" s="4" t="n">
+      <c r="H14" s="2" t="n">
         <v>0.971333333333333</v>
       </c>
-      <c r="I14" s="4" t="n">
+      <c r="I14" s="2" t="n">
         <v>0.928994082840236</v>
       </c>
-      <c r="J14" s="4" t="n">
+      <c r="J14" s="2" t="n">
         <v>0.8785</v>
       </c>
-      <c r="K14" s="4" t="n">
+      <c r="K14" s="2" t="n">
         <v>0.838</v>
       </c>
-      <c r="L14" s="4" t="n">
+      <c r="L14" s="2" t="n">
         <v>0.95655423264967</v>
       </c>
-      <c r="M14" s="4" t="n">
+      <c r="M14" s="2" t="n">
         <v>0.99474</v>
       </c>
-      <c r="N14" s="0" t="n">
+      <c r="N14" s="1" t="n">
         <v>100</v>
       </c>
     </row>
@@ -592,31 +587,31 @@
       <c r="E15" s="0" t="n">
         <v>2592</v>
       </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="2" t="n">
         <v>0.676354029062087</v>
       </c>
-      <c r="G15" s="4" t="n">
+      <c r="G15" s="2" t="n">
         <v>0.441379310344828</v>
       </c>
-      <c r="H15" s="4" t="n">
+      <c r="H15" s="2" t="n">
         <v>0.973185947247455</v>
       </c>
-      <c r="I15" s="4" t="n">
+      <c r="I15" s="2" t="n">
         <v>0.534167970787689</v>
       </c>
-      <c r="J15" s="4" t="n">
+      <c r="J15" s="2" t="n">
         <v>0.913275711372244</v>
       </c>
-      <c r="K15" s="4" t="n">
+      <c r="K15" s="2" t="n">
         <v>0.488674566783753</v>
       </c>
-      <c r="L15" s="4" t="n">
+      <c r="L15" s="2" t="n">
         <v>0.655396171970328</v>
       </c>
-      <c r="M15" s="4" t="n">
+      <c r="M15" s="2" t="n">
         <v>0.942780647108385</v>
       </c>
-      <c r="N15" s="0" t="n">
+      <c r="N15" s="1" t="n">
         <v>100</v>
       </c>
     </row>
@@ -636,31 +631,31 @@
       <c r="E16" s="0" t="n">
         <v>8764</v>
       </c>
-      <c r="F16" s="4" t="n">
+      <c r="F16" s="2" t="n">
         <v>0.622757673738761</v>
       </c>
-      <c r="G16" s="4" t="n">
+      <c r="G16" s="2" t="n">
         <v>0.616018226428321</v>
       </c>
-      <c r="H16" s="4" t="n">
+      <c r="H16" s="2" t="n">
         <v>0.73598065656096</v>
       </c>
-      <c r="I16" s="4" t="n">
+      <c r="I16" s="2" t="n">
         <v>0.619369617409308</v>
       </c>
-      <c r="J16" s="4" t="n">
+      <c r="J16" s="2" t="n">
         <v>0.686273441896774</v>
       </c>
-      <c r="K16" s="4" t="n">
+      <c r="K16" s="2" t="n">
         <v>0.352556833062971</v>
       </c>
-      <c r="L16" s="4" t="n">
+      <c r="L16" s="2" t="n">
         <v>0.673333126127204</v>
       </c>
-      <c r="M16" s="4" t="n">
+      <c r="M16" s="2" t="n">
         <v>0.741831872697634</v>
       </c>
-      <c r="N16" s="0" t="n">
+      <c r="N16" s="1" t="n">
         <v>100</v>
       </c>
     </row>
@@ -709,7 +704,7 @@
       <c r="M21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N21" s="0" t="s">
+      <c r="N21" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -717,40 +712,40 @@
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="2" t="n">
+      <c r="B22" s="0" t="n">
         <v>508</v>
       </c>
-      <c r="C22" s="2" t="n">
+      <c r="C22" s="0" t="n">
         <v>410</v>
       </c>
-      <c r="D22" s="2" t="n">
+      <c r="D22" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E22" s="2" t="n">
+      <c r="E22" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F22" s="3" t="n">
+      <c r="F22" s="2" t="n">
         <v>0.553376906318083</v>
       </c>
-      <c r="G22" s="3" t="n">
+      <c r="G22" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H22" s="3" t="n">
+      <c r="H22" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I22" s="3" t="n">
+      <c r="I22" s="2" t="n">
         <v>0.712482468443198</v>
       </c>
-      <c r="J22" s="3" t="n">
+      <c r="J22" s="2" t="n">
         <v>0.553376906318083</v>
       </c>
-      <c r="K22" s="3" t="n">
+      <c r="K22" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L22" s="3" t="n">
+      <c r="L22" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M22" s="3" t="n">
+      <c r="M22" s="2" t="n">
         <v>0.481904167466871</v>
       </c>
     </row>
@@ -770,28 +765,28 @@
       <c r="E23" s="0" t="n">
         <v>312</v>
       </c>
-      <c r="F23" s="4" t="n">
+      <c r="F23" s="2" t="n">
         <v>0.235</v>
       </c>
-      <c r="G23" s="4" t="n">
+      <c r="G23" s="2" t="n">
         <v>0.376</v>
       </c>
-      <c r="H23" s="4" t="n">
+      <c r="H23" s="2" t="n">
         <v>0.592</v>
       </c>
-      <c r="I23" s="4" t="n">
+      <c r="I23" s="2" t="n">
         <v>0.289230769230769</v>
       </c>
-      <c r="J23" s="4" t="n">
+      <c r="J23" s="2" t="n">
         <v>0.233</v>
       </c>
-      <c r="K23" s="4" t="n">
+      <c r="K23" s="2" t="n">
         <v>-0.0226666666666666</v>
       </c>
-      <c r="L23" s="4" t="n">
+      <c r="L23" s="2" t="n">
         <v>0.471796566329175</v>
       </c>
-      <c r="M23" s="4" t="n">
+      <c r="M23" s="2" t="n">
         <v>0.478666666666667</v>
       </c>
     </row>
@@ -811,24 +806,24 @@
       <c r="E24" s="0" t="n">
         <v>4640</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4" t="n">
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="H24" s="4" t="n">
+      <c r="H24" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4" t="n">
+      <c r="I24" s="2"/>
+      <c r="J24" s="2" t="n">
         <v>0.887345828882199</v>
       </c>
-      <c r="K24" s="4" t="n">
+      <c r="K24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L24" s="4" t="n">
+      <c r="L24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M24" s="4" t="n">
+      <c r="M24" s="2" t="n">
         <v>0.489205288722813</v>
       </c>
     </row>
@@ -848,24 +843,24 @@
       <c r="E25" s="0" t="n">
         <v>22824</v>
       </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4" t="n">
+      <c r="F25" s="2"/>
+      <c r="G25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="H25" s="4" t="n">
+      <c r="H25" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4" t="n">
+      <c r="I25" s="2"/>
+      <c r="J25" s="2" t="n">
         <v>0.585643483470399</v>
       </c>
-      <c r="K25" s="4" t="n">
+      <c r="K25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L25" s="4" t="n">
+      <c r="L25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M25" s="4" t="n">
+      <c r="M25" s="2" t="n">
         <v>0.497372780689009</v>
       </c>
     </row>
@@ -914,7 +909,7 @@
       <c r="M30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N30" s="0" t="s">
+      <c r="N30" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -922,43 +917,43 @@
       <c r="A31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="2" t="n">
+      <c r="B31" s="0" t="n">
         <v>436</v>
       </c>
-      <c r="C31" s="2" t="n">
+      <c r="C31" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="D31" s="2" t="n">
+      <c r="D31" s="0" t="n">
         <v>335</v>
       </c>
-      <c r="E31" s="2" t="n">
+      <c r="E31" s="0" t="n">
         <v>72</v>
       </c>
-      <c r="F31" s="3" t="n">
+      <c r="F31" s="2" t="n">
         <v>0.853228962818004</v>
       </c>
-      <c r="G31" s="3" t="n">
+      <c r="G31" s="2" t="n">
         <v>0.858267716535433</v>
       </c>
-      <c r="H31" s="3" t="n">
+      <c r="H31" s="2" t="n">
         <v>0.817073170731707</v>
       </c>
-      <c r="I31" s="3" t="n">
+      <c r="I31" s="2" t="n">
         <v>0.855740922473013</v>
       </c>
-      <c r="J31" s="3" t="n">
+      <c r="J31" s="2" t="n">
         <v>0.839869281045752</v>
       </c>
-      <c r="K31" s="3" t="n">
+      <c r="K31" s="2" t="n">
         <v>0.675817866460388</v>
       </c>
-      <c r="L31" s="3" t="n">
+      <c r="L31" s="2" t="n">
         <v>0.837417174702232</v>
       </c>
-      <c r="M31" s="3" t="n">
+      <c r="M31" s="2" t="n">
         <v>0.91519589014788</v>
       </c>
-      <c r="N31" s="0" t="n">
+      <c r="N31" s="1" t="n">
         <v>22</v>
       </c>
     </row>
@@ -978,31 +973,31 @@
       <c r="E32" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="F32" s="4" t="n">
+      <c r="F32" s="2" t="n">
         <v>0.866799204771372</v>
       </c>
-      <c r="G32" s="4" t="n">
+      <c r="G32" s="2" t="n">
         <v>0.872</v>
       </c>
-      <c r="H32" s="4" t="n">
+      <c r="H32" s="2" t="n">
         <v>0.955333333333333</v>
       </c>
-      <c r="I32" s="4" t="n">
+      <c r="I32" s="2" t="n">
         <v>0.869391824526421</v>
       </c>
-      <c r="J32" s="4" t="n">
+      <c r="J32" s="2" t="n">
         <v>0.789</v>
       </c>
-      <c r="K32" s="4" t="n">
+      <c r="K32" s="2" t="n">
         <v>0.718666666666667</v>
       </c>
-      <c r="L32" s="4" t="n">
+      <c r="L32" s="2" t="n">
         <v>0.912716093134479</v>
       </c>
-      <c r="M32" s="4" t="n">
+      <c r="M32" s="2" t="n">
         <v>0.979565333333335</v>
       </c>
-      <c r="N32" s="0" t="n">
+      <c r="N32" s="1" t="n">
         <v>80</v>
       </c>
     </row>
@@ -1022,31 +1017,31 @@
       <c r="E33" s="0" t="n">
         <v>2129</v>
       </c>
-      <c r="F33" s="4" t="n">
+      <c r="F33" s="2" t="n">
         <v>0.411302211302211</v>
       </c>
-      <c r="G33" s="4" t="n">
+      <c r="G33" s="2" t="n">
         <v>0.541163793103448</v>
       </c>
-      <c r="H33" s="4" t="n">
+      <c r="H33" s="2" t="n">
         <v>0.90166356572179</v>
       </c>
-      <c r="I33" s="4" t="n">
+      <c r="I33" s="2" t="n">
         <v>0.467380176826431</v>
       </c>
-      <c r="J33" s="4" t="n">
+      <c r="J33" s="2" t="n">
         <v>0.861051762649315</v>
       </c>
-      <c r="K33" s="4" t="n">
+      <c r="K33" s="2" t="n">
         <v>0.389187839485958</v>
       </c>
-      <c r="L33" s="4" t="n">
+      <c r="L33" s="2" t="n">
         <v>0.698532515584768</v>
       </c>
-      <c r="M33" s="4" t="n">
+      <c r="M33" s="2" t="n">
         <v>0.833570018218757</v>
       </c>
-      <c r="N33" s="0" t="n">
+      <c r="N33" s="1" t="n">
         <v>40</v>
       </c>
     </row>
@@ -1066,31 +1061,31 @@
       <c r="E34" s="0" t="n">
         <v>6675</v>
       </c>
-      <c r="F34" s="4" t="n">
+      <c r="F34" s="2" t="n">
         <v>0.735315545032328</v>
       </c>
-      <c r="G34" s="4" t="n">
+      <c r="G34" s="2" t="n">
         <v>0.70754468980021</v>
       </c>
-      <c r="H34" s="4" t="n">
+      <c r="H34" s="2" t="n">
         <v>0.819802225735454</v>
       </c>
-      <c r="I34" s="4" t="n">
+      <c r="I34" s="2" t="n">
         <v>0.721162863394811</v>
       </c>
-      <c r="J34" s="4" t="n">
+      <c r="J34" s="2" t="n">
         <v>0.77328758419113</v>
       </c>
-      <c r="K34" s="4" t="n">
+      <c r="K34" s="2" t="n">
         <v>0.530275637811701</v>
       </c>
-      <c r="L34" s="4" t="n">
+      <c r="L34" s="2" t="n">
         <v>0.761607977574758</v>
       </c>
-      <c r="M34" s="4" t="n">
+      <c r="M34" s="2" t="n">
         <v>0.84888718795856</v>
       </c>
-      <c r="N34" s="0" t="n">
+      <c r="N34" s="1" t="n">
         <v>117</v>
       </c>
     </row>
@@ -1139,7 +1134,7 @@
       <c r="M39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N39" s="0" t="s">
+      <c r="N39" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1147,43 +1142,43 @@
       <c r="A40" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="2" t="n">
-        <v>372</v>
-      </c>
-      <c r="C40" s="2" t="n">
-        <v>116</v>
-      </c>
-      <c r="D40" s="2" t="n">
-        <v>294</v>
-      </c>
-      <c r="E40" s="2" t="n">
-        <v>136</v>
-      </c>
-      <c r="F40" s="3" t="n">
-        <v>0.762295081967213</v>
-      </c>
-      <c r="G40" s="3" t="n">
-        <v>0.732283464566929</v>
-      </c>
-      <c r="H40" s="3" t="n">
-        <v>0.717073170731707</v>
-      </c>
-      <c r="I40" s="3" t="n">
-        <v>0.746987951807229</v>
-      </c>
-      <c r="J40" s="3" t="n">
-        <v>0.725490196078431</v>
-      </c>
-      <c r="K40" s="3" t="n">
-        <v>0.447252222116028</v>
-      </c>
-      <c r="L40" s="3" t="n">
-        <v>0.724638410389214</v>
-      </c>
-      <c r="M40" s="3" t="n">
-        <v>0.783181294411372</v>
-      </c>
-      <c r="N40" s="0" t="n">
+      <c r="B40" s="0" t="n">
+        <v>449</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>339</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="F40" s="2" t="n">
+        <v>0.863461538461539</v>
+      </c>
+      <c r="G40" s="2" t="n">
+        <v>0.883858267716535</v>
+      </c>
+      <c r="H40" s="2" t="n">
+        <v>0.826829268292683</v>
+      </c>
+      <c r="I40" s="2" t="n">
+        <v>0.873540856031128</v>
+      </c>
+      <c r="J40" s="2" t="n">
+        <v>0.85838779956427</v>
+      </c>
+      <c r="K40" s="2" t="n">
+        <v>0.71269957436974</v>
+      </c>
+      <c r="L40" s="2" t="n">
+        <v>0.854868343530453</v>
+      </c>
+      <c r="M40" s="2" t="n">
+        <v>0.924087766468219</v>
+      </c>
+      <c r="N40" s="1" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1192,42 +1187,42 @@
         <v>16</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>173</v>
+        <v>450</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>326</v>
+        <v>55</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>1174</v>
+        <v>1445</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>327</v>
-      </c>
-      <c r="F41" s="4" t="n">
-        <v>0.346693386773547</v>
-      </c>
-      <c r="G41" s="4" t="n">
-        <v>0.346</v>
-      </c>
-      <c r="H41" s="4" t="n">
-        <v>0.782666666666667</v>
-      </c>
-      <c r="I41" s="4" t="n">
-        <v>0.346346346346346</v>
-      </c>
-      <c r="J41" s="4" t="n">
-        <v>0.321</v>
-      </c>
-      <c r="K41" s="4" t="n">
-        <v>0.0946666666666667</v>
-      </c>
-      <c r="L41" s="4" t="n">
-        <v>0.52038703545214</v>
-      </c>
-      <c r="M41" s="4" t="n">
-        <v>0.610853333333334</v>
-      </c>
-      <c r="N41" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <v>0.891089108910891</v>
+      </c>
+      <c r="G41" s="2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="H41" s="2" t="n">
+        <v>0.963333333333333</v>
+      </c>
+      <c r="I41" s="2" t="n">
+        <v>0.895522388059701</v>
+      </c>
+      <c r="J41" s="2" t="n">
+        <v>0.7555</v>
+      </c>
+      <c r="K41" s="2" t="n">
+        <v>0.674</v>
+      </c>
+      <c r="L41" s="2" t="n">
+        <v>0.931128347758782</v>
+      </c>
+      <c r="M41" s="2" t="n">
+        <v>0.986253333333333</v>
+      </c>
+      <c r="N41" s="1" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1236,42 +1231,42 @@
         <v>17</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>2174</v>
+        <v>1709</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>1415</v>
+        <v>935</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>35133</v>
+        <v>35613</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>2466</v>
-      </c>
-      <c r="F42" s="4" t="n">
-        <v>0.605739760378936</v>
-      </c>
-      <c r="G42" s="4" t="n">
-        <v>0.468534482758621</v>
-      </c>
-      <c r="H42" s="4" t="n">
-        <v>0.961283791178724</v>
-      </c>
-      <c r="I42" s="4" t="n">
-        <v>0.528375258233078</v>
-      </c>
-      <c r="J42" s="4" t="n">
-        <v>0.905773526269787</v>
-      </c>
-      <c r="K42" s="4" t="n">
-        <v>0.476980142782518</v>
-      </c>
-      <c r="L42" s="4" t="n">
-        <v>0.671114449169566</v>
-      </c>
-      <c r="M42" s="4" t="n">
-        <v>0.878503877045856</v>
-      </c>
-      <c r="N42" s="0" t="n">
+        <v>2931</v>
+      </c>
+      <c r="F42" s="2" t="n">
+        <v>0.646369137670197</v>
+      </c>
+      <c r="G42" s="2" t="n">
+        <v>0.368318965517241</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <v>0.974417204771807</v>
+      </c>
+      <c r="I42" s="2" t="n">
+        <v>0.469247666117518</v>
+      </c>
+      <c r="J42" s="2" t="n">
+        <v>0.906137710012625</v>
+      </c>
+      <c r="K42" s="2" t="n">
+        <v>0.421974370338886</v>
+      </c>
+      <c r="L42" s="2" t="n">
+        <v>0.599079574717544</v>
+      </c>
+      <c r="M42" s="2" t="n">
+        <v>0.923931922426989</v>
+      </c>
+      <c r="N42" s="1" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1280,42 +1275,42 @@
         <v>18</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>16536</v>
+        <v>11718</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>4366</v>
+        <v>5447</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>27893</v>
+        <v>26812</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>6288</v>
-      </c>
-      <c r="F43" s="4" t="n">
-        <v>0.791120466940963</v>
-      </c>
-      <c r="G43" s="4" t="n">
-        <v>0.724500525762355</v>
-      </c>
-      <c r="H43" s="4" t="n">
-        <v>0.864657924920177</v>
-      </c>
-      <c r="I43" s="4" t="n">
-        <v>0.756346338562869</v>
-      </c>
-      <c r="J43" s="4" t="n">
-        <v>0.806582793239293</v>
-      </c>
-      <c r="K43" s="4" t="n">
-        <v>0.596504200607112</v>
-      </c>
-      <c r="L43" s="4" t="n">
-        <v>0.791482862233451</v>
-      </c>
-      <c r="M43" s="4" t="n">
-        <v>0.874645775103436</v>
-      </c>
-      <c r="N43" s="0" t="n">
+        <v>11106</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <v>0.682668220215555</v>
+      </c>
+      <c r="G43" s="2" t="n">
+        <v>0.513406940063091</v>
+      </c>
+      <c r="H43" s="2" t="n">
+        <v>0.831147896710995</v>
+      </c>
+      <c r="I43" s="2" t="n">
+        <v>0.586061166820876</v>
+      </c>
+      <c r="J43" s="2" t="n">
+        <v>0.699489860755587</v>
+      </c>
+      <c r="K43" s="2" t="n">
+        <v>0.357517871971648</v>
+      </c>
+      <c r="L43" s="2" t="n">
+        <v>0.653235867348285</v>
+      </c>
+      <c r="M43" s="2" t="n">
+        <v>0.74217206623632</v>
+      </c>
+      <c r="N43" s="1" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1364,7 +1359,7 @@
       <c r="M48" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N48" s="0" t="s">
+      <c r="N48" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1372,43 +1367,43 @@
       <c r="A49" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="2" t="n">
+      <c r="B49" s="0" t="n">
         <v>450</v>
       </c>
-      <c r="C49" s="2" t="n">
-        <v>83</v>
-      </c>
-      <c r="D49" s="2" t="n">
-        <v>327</v>
-      </c>
-      <c r="E49" s="2" t="n">
+      <c r="C49" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>324</v>
+      </c>
+      <c r="E49" s="0" t="n">
         <v>58</v>
       </c>
-      <c r="F49" s="3" t="n">
-        <v>0.844277673545966</v>
-      </c>
-      <c r="G49" s="3" t="n">
+      <c r="F49" s="2" t="n">
+        <v>0.83955223880597</v>
+      </c>
+      <c r="G49" s="2" t="n">
         <v>0.885826771653543</v>
       </c>
-      <c r="H49" s="3" t="n">
-        <v>0.797560975609756</v>
-      </c>
-      <c r="I49" s="3" t="n">
-        <v>0.864553314121037</v>
-      </c>
-      <c r="J49" s="3" t="n">
-        <v>0.84640522875817</v>
-      </c>
-      <c r="K49" s="3" t="n">
-        <v>0.687430875854242</v>
-      </c>
-      <c r="L49" s="3" t="n">
-        <v>0.840536057656803</v>
-      </c>
-      <c r="M49" s="3" t="n">
-        <v>0.84169387363165</v>
-      </c>
-      <c r="N49" s="0" t="n">
+      <c r="H49" s="2" t="n">
+        <v>0.790243902439024</v>
+      </c>
+      <c r="I49" s="2" t="n">
+        <v>0.862068965517241</v>
+      </c>
+      <c r="J49" s="2" t="n">
+        <v>0.843137254901961</v>
+      </c>
+      <c r="K49" s="2" t="n">
+        <v>0.680553676029926</v>
+      </c>
+      <c r="L49" s="2" t="n">
+        <v>0.836671503588152</v>
+      </c>
+      <c r="M49" s="2" t="n">
+        <v>0.838035337046284</v>
+      </c>
+      <c r="N49" s="1" t="n">
         <v>735</v>
       </c>
     </row>
@@ -1416,43 +1411,43 @@
       <c r="A50" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B50" s="1" t="n">
-        <v>233</v>
-      </c>
-      <c r="C50" s="1" t="n">
-        <v>243</v>
-      </c>
-      <c r="D50" s="1" t="n">
-        <v>1257</v>
-      </c>
-      <c r="E50" s="1" t="n">
-        <v>267</v>
-      </c>
-      <c r="F50" s="3" t="n">
-        <v>0.489495798319328</v>
-      </c>
-      <c r="G50" s="3" t="n">
-        <v>0.466</v>
-      </c>
-      <c r="H50" s="3" t="n">
-        <v>0.838</v>
-      </c>
-      <c r="I50" s="3" t="n">
-        <v>0.477459016393443</v>
-      </c>
-      <c r="J50" s="3" t="n">
-        <v>0.3705</v>
-      </c>
-      <c r="K50" s="3" t="n">
-        <v>0.160666666666667</v>
-      </c>
-      <c r="L50" s="3" t="n">
-        <v>0.624906392990182</v>
-      </c>
-      <c r="M50" s="3" t="n">
-        <v>0.745064666666667</v>
-      </c>
-      <c r="N50" s="0" t="n">
+      <c r="B50" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>187</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>1313</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="F50" s="2" t="n">
+        <v>0.616016427104723</v>
+      </c>
+      <c r="G50" s="2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H50" s="2" t="n">
+        <v>0.875333333333333</v>
+      </c>
+      <c r="I50" s="2" t="n">
+        <v>0.60790273556231</v>
+      </c>
+      <c r="J50" s="2" t="n">
+        <v>0.4765</v>
+      </c>
+      <c r="K50" s="2" t="n">
+        <v>0.302</v>
+      </c>
+      <c r="L50" s="2" t="n">
+        <v>0.724706837279738</v>
+      </c>
+      <c r="M50" s="2" t="n">
+        <v>0.843209333333333</v>
+      </c>
+      <c r="N50" s="1" t="n">
         <v>1600</v>
       </c>
     </row>
@@ -1461,42 +1456,42 @@
         <v>17</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>1488</v>
+        <v>1992</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>1310</v>
+        <v>1638</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>35238</v>
+        <v>34910</v>
       </c>
       <c r="E51" s="0" t="n">
-        <v>3152</v>
-      </c>
-      <c r="F51" s="4" t="n">
-        <v>0.53180843459614</v>
-      </c>
-      <c r="G51" s="4" t="n">
-        <v>0.320689655172414</v>
-      </c>
-      <c r="H51" s="4" t="n">
-        <v>0.964156725402211</v>
-      </c>
-      <c r="I51" s="4" t="n">
-        <v>0.400107555794568</v>
-      </c>
-      <c r="J51" s="4" t="n">
-        <v>0.891667475963873</v>
-      </c>
-      <c r="K51" s="4" t="n">
-        <v>0.344554857599803</v>
-      </c>
-      <c r="L51" s="4" t="n">
-        <v>0.556053133973183</v>
-      </c>
-      <c r="M51" s="4" t="n">
-        <v>0.751742665762172</v>
-      </c>
-      <c r="N51" s="0" t="n">
+        <v>2648</v>
+      </c>
+      <c r="F51" s="2" t="n">
+        <v>0.548760330578512</v>
+      </c>
+      <c r="G51" s="2" t="n">
+        <v>0.429310344827586</v>
+      </c>
+      <c r="H51" s="2" t="n">
+        <v>0.955182226113604</v>
+      </c>
+      <c r="I51" s="2" t="n">
+        <v>0.48174123337364</v>
+      </c>
+      <c r="J51" s="2" t="n">
+        <v>0.895940565213169</v>
+      </c>
+      <c r="K51" s="2" t="n">
+        <v>0.424862477273939</v>
+      </c>
+      <c r="L51" s="2" t="n">
+        <v>0.640366778390332</v>
+      </c>
+      <c r="M51" s="2" t="n">
+        <v>0.819059229619622</v>
+      </c>
+      <c r="N51" s="1" t="n">
         <v>32951</v>
       </c>
     </row>
@@ -1504,43 +1499,43 @@
       <c r="A52" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B52" s="0" t="n">
-        <v>16702</v>
-      </c>
-      <c r="C52" s="0" t="n">
-        <v>4670</v>
-      </c>
-      <c r="D52" s="0" t="n">
-        <v>27589</v>
-      </c>
-      <c r="E52" s="0" t="n">
-        <v>6122</v>
-      </c>
-      <c r="F52" s="4" t="n">
-        <v>0.781489799737975</v>
-      </c>
-      <c r="G52" s="4" t="n">
-        <v>0.731773571678934</v>
-      </c>
-      <c r="H52" s="4" t="n">
-        <v>0.855234198208252</v>
-      </c>
-      <c r="I52" s="4" t="n">
-        <v>0.755815005882885</v>
-      </c>
-      <c r="J52" s="4" t="n">
-        <v>0.804077483071002</v>
-      </c>
-      <c r="K52" s="4" t="n">
-        <v>0.592520147859203</v>
-      </c>
-      <c r="L52" s="4" t="n">
-        <v>0.791099098624706</v>
-      </c>
-      <c r="M52" s="4" t="n">
-        <v>0.855471713336612</v>
-      </c>
-      <c r="N52" s="0" t="n">
+      <c r="B52" s="1" t="n">
+        <v>16889</v>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>4585</v>
+      </c>
+      <c r="D52" s="1" t="n">
+        <v>27674</v>
+      </c>
+      <c r="E52" s="1" t="n">
+        <v>5935</v>
+      </c>
+      <c r="F52" s="3" t="n">
+        <v>0.786485983049269</v>
+      </c>
+      <c r="G52" s="3" t="n">
+        <v>0.73996670171749</v>
+      </c>
+      <c r="H52" s="3" t="n">
+        <v>0.857869121795468</v>
+      </c>
+      <c r="I52" s="3" t="n">
+        <v>0.762517495146508</v>
+      </c>
+      <c r="J52" s="3" t="n">
+        <v>0.809015485721547</v>
+      </c>
+      <c r="K52" s="3" t="n">
+        <v>0.60305206667372</v>
+      </c>
+      <c r="L52" s="3" t="n">
+        <v>0.796739972990104</v>
+      </c>
+      <c r="M52" s="3" t="n">
+        <v>0.859904716526803</v>
+      </c>
+      <c r="N52" s="1" t="n">
         <v>44067</v>
       </c>
     </row>

</xml_diff>